<commit_message>
small update to baseline boundaries
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_BaselineBoundaries.xlsx
+++ b/SuppXLS/Scen_ELC_BaselineBoundaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1C394D-D6A1-425E-8428-5DD860953C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CDD68F-4B71-47A6-8D52-10B757FE7CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16680" yWindow="456" windowWidth="23412" windowHeight="15888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="24">
   <si>
     <t>Pset_PN</t>
   </si>
@@ -578,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AE42"/>
+  <dimension ref="C2:AE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +784,7 @@
       </c>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C14" s="12"/>
       <c r="D14" s="12">
         <v>2045</v>
@@ -814,11 +814,11 @@
       </c>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="15">
-        <v>2015</v>
-      </c>
-      <c r="E15" s="15" t="s">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D15" s="12">
+        <v>2050</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -826,28 +826,28 @@
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="15">
-        <v>0</v>
-      </c>
-      <c r="J15" s="15">
-        <v>0</v>
-      </c>
-      <c r="K15" s="15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>21</v>
+      <c r="I15" s="12">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="8"/>
-      <c r="D16" s="15">
-        <v>2020</v>
-      </c>
-      <c r="E16" s="15" t="s">
+      <c r="D16" s="12">
+        <v>2050</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="12" t="s">
@@ -855,26 +855,26 @@
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="15">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15">
-        <v>0</v>
-      </c>
-      <c r="K16" s="15">
-        <v>0</v>
-      </c>
-      <c r="L16" s="15">
-        <v>0</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>21</v>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="13">
+        <v>0</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="4:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="15">
-        <v>2025</v>
+        <v>2015</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>20</v>
@@ -882,6 +882,8 @@
       <c r="F17" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="15">
         <v>0</v>
       </c>
@@ -912,7 +914,7 @@
     </row>
     <row r="18" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" s="15">
-        <v>2010</v>
+        <v>2020</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>20</v>
@@ -920,6 +922,8 @@
       <c r="F18" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="15">
         <v>0</v>
       </c>
@@ -932,8 +936,8 @@
       <c r="L18" s="15">
         <v>0</v>
       </c>
-      <c r="M18" s="12" t="s">
-        <v>22</v>
+      <c r="M18" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="T18" s="10" t="s">
         <v>8</v>
@@ -974,7 +978,7 @@
     </row>
     <row r="19" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D19" s="15">
-        <v>2015</v>
+        <v>2025</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>20</v>
@@ -994,9 +998,8 @@
       <c r="L19" s="15">
         <v>0</v>
       </c>
-      <c r="M19" s="12" t="str">
-        <f>M18</f>
-        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
+      <c r="M19" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="U19">
         <v>2030</v>
@@ -1013,7 +1016,7 @@
     </row>
     <row r="20" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D20" s="15">
-        <v>2020</v>
+        <v>2010</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>20</v>
@@ -1033,9 +1036,8 @@
       <c r="L20" s="15">
         <v>0</v>
       </c>
-      <c r="M20" s="12" t="str">
-        <f>M19</f>
-        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
+      <c r="M20" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="U20">
         <v>2030</v>
@@ -1052,7 +1054,7 @@
     </row>
     <row r="21" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D21" s="15">
-        <v>2030</v>
+        <v>2015</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>20</v>
@@ -1073,120 +1075,121 @@
         <v>0</v>
       </c>
       <c r="M21" s="12" t="str">
-        <f t="shared" ref="M21:M23" si="0">M20</f>
+        <f>M20</f>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
     <row r="22" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D22" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="15">
+        <v>0</v>
+      </c>
+      <c r="K22" s="15">
+        <v>0</v>
+      </c>
+      <c r="L22" s="15">
+        <v>0</v>
+      </c>
+      <c r="M22" s="12" t="str">
+        <f>M21</f>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="23" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D23" s="15">
+        <v>2030</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15">
+        <v>0</v>
+      </c>
+      <c r="K23" s="15">
+        <v>0</v>
+      </c>
+      <c r="L23" s="15">
+        <v>0</v>
+      </c>
+      <c r="M23" s="12" t="str">
+        <f t="shared" ref="M23:M25" si="0">M22</f>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
+      </c>
+    </row>
+    <row r="24" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D24" s="15">
         <v>2040</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="15">
-        <v>0</v>
-      </c>
-      <c r="J22" s="15">
-        <v>0</v>
-      </c>
-      <c r="K22" s="15">
-        <v>0</v>
-      </c>
-      <c r="L22" s="15">
-        <v>0</v>
-      </c>
-      <c r="M22" s="12" t="str">
+      <c r="E24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="15">
+        <v>0</v>
+      </c>
+      <c r="J24" s="15">
+        <v>0</v>
+      </c>
+      <c r="K24" s="15">
+        <v>0</v>
+      </c>
+      <c r="L24" s="15">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12" t="str">
         <f t="shared" si="0"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="23" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D23" s="15">
+    <row r="25" spans="4:31" x14ac:dyDescent="0.3">
+      <c r="D25" s="15">
         <v>2050</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="15">
-        <v>0</v>
-      </c>
-      <c r="J23" s="15">
-        <v>0</v>
-      </c>
-      <c r="K23" s="15">
-        <v>0</v>
-      </c>
-      <c r="L23" s="15">
-        <v>0</v>
-      </c>
-      <c r="M23" s="12" t="str">
+      <c r="E25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="15">
+        <v>0</v>
+      </c>
+      <c r="J25" s="15">
+        <v>0</v>
+      </c>
+      <c r="K25" s="15">
+        <v>0</v>
+      </c>
+      <c r="L25" s="15">
+        <v>0</v>
+      </c>
+      <c r="M25" s="12" t="str">
         <f t="shared" si="0"/>
         <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
-    <row r="24" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D24" s="15">
-        <v>2010</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="15">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15">
-        <v>0</v>
-      </c>
-      <c r="K24" s="15">
-        <v>0</v>
-      </c>
-      <c r="L24" s="15">
-        <v>0</v>
-      </c>
-      <c r="M24" s="12" t="str">
-        <f>M20</f>
-        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
-      </c>
-    </row>
-    <row r="25" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D25" s="15">
-        <v>2015</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="15">
-        <v>0</v>
-      </c>
-      <c r="J25" s="15">
-        <v>0</v>
-      </c>
-      <c r="K25" s="15">
-        <v>0</v>
-      </c>
-      <c r="L25" s="15">
-        <v>0</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="26" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D26" s="15">
-        <v>2020</v>
+        <v>2010</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>20</v>
@@ -1207,13 +1210,13 @@
         <v>0</v>
       </c>
       <c r="M26" s="12" t="str">
-        <f>M25</f>
-        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
+        <f>M22</f>
+        <v>TB_SUPCO2_DKISLBH_DKE_01</v>
       </c>
     </row>
     <row r="27" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D27" s="15">
-        <v>2025</v>
+        <v>2015</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>20</v>
@@ -1233,14 +1236,13 @@
       <c r="L27" s="15">
         <v>0</v>
       </c>
-      <c r="M27" s="12" t="str">
-        <f t="shared" ref="M27:M30" si="1">M26</f>
-        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
+      <c r="M27" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D28" s="15">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>20</v>
@@ -1261,13 +1263,13 @@
         <v>0</v>
       </c>
       <c r="M28" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f>M27</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="29" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D29" s="15">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>20</v>
@@ -1288,13 +1290,13 @@
         <v>0</v>
       </c>
       <c r="M29" s="12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="M29:M32" si="1">M28</f>
         <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="30" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D30" s="15">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>20</v>
@@ -1321,7 +1323,7 @@
     </row>
     <row r="31" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D31" s="15">
-        <v>2015</v>
+        <v>2040</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>20</v>
@@ -1341,13 +1343,14 @@
       <c r="L31" s="15">
         <v>0</v>
       </c>
-      <c r="M31" s="12" t="s">
-        <v>11</v>
+      <c r="M31" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="32" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D32" s="15">
-        <v>2020</v>
+        <v>2050</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>20</v>
@@ -1367,13 +1370,14 @@
       <c r="L32" s="15">
         <v>0</v>
       </c>
-      <c r="M32" s="12" t="s">
-        <v>11</v>
+      <c r="M32" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_SUPCO2_DKISLBH_DKE_02</v>
       </c>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D33" s="15">
-        <v>2025</v>
+        <v>2015</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>20</v>
@@ -1399,7 +1403,7 @@
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D34" s="15">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>20</v>
@@ -1420,12 +1424,12 @@
         <v>0</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D35" s="15">
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>20</v>
@@ -1446,12 +1450,12 @@
         <v>0</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D36" s="15">
-        <v>2025</v>
+        <v>2015</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>20</v>
@@ -1477,16 +1481,13 @@
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D37" s="15">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
+      <c r="F37" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="I37" s="15">
         <v>0</v>
@@ -1500,22 +1501,19 @@
       <c r="L37" s="15">
         <v>0</v>
       </c>
-      <c r="M37" s="15" t="s">
-        <v>17</v>
+      <c r="M37" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D38" s="15">
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
+      <c r="F38" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="I38" s="15">
         <v>0</v>
@@ -1529,13 +1527,13 @@
       <c r="L38" s="15">
         <v>0</v>
       </c>
-      <c r="M38" s="15" t="s">
-        <v>17</v>
+      <c r="M38" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D39" s="15">
-        <v>2025</v>
+        <v>2015</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>20</v>
@@ -1564,7 +1562,7 @@
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D40" s="15">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>20</v>
@@ -1572,7 +1570,7 @@
       <c r="F40" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H40">
+      <c r="G40">
         <v>0</v>
       </c>
       <c r="I40" s="15">
@@ -1588,12 +1586,12 @@
         <v>0</v>
       </c>
       <c r="M40" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.3">
       <c r="D41" s="15">
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="E41" s="15" t="s">
         <v>20</v>
@@ -1601,7 +1599,7 @@
       <c r="F41" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H41">
+      <c r="G41">
         <v>0</v>
       </c>
       <c r="I41" s="15">
@@ -1617,13 +1615,13 @@
         <v>0</v>
       </c>
       <c r="M41" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C42" s="12"/>
       <c r="D42" s="15">
-        <v>2025</v>
+        <v>2015</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>20</v>
@@ -1647,6 +1645,64 @@
         <v>0</v>
       </c>
       <c r="M42" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="D43" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" s="15">
+        <v>0</v>
+      </c>
+      <c r="J43" s="15">
+        <v>0</v>
+      </c>
+      <c r="K43" s="15">
+        <v>0</v>
+      </c>
+      <c r="L43" s="15">
+        <v>0</v>
+      </c>
+      <c r="M43" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="D44" s="15">
+        <v>2025</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44" s="15">
+        <v>0</v>
+      </c>
+      <c r="J44" s="15">
+        <v>0</v>
+      </c>
+      <c r="K44" s="15">
+        <v>0</v>
+      </c>
+      <c r="L44" s="15">
+        <v>0</v>
+      </c>
+      <c r="M44" s="15" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>